<commit_message>
Updating Sprint 31 test cases
</commit_message>
<xml_diff>
--- a/TestData/IMIassist_Automation_TestData (1).xlsx
+++ b/TestData/IMIassist_Automation_TestData (1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Login_testdata" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="141">
   <si>
     <t>URL</t>
   </si>
@@ -439,6 +439,27 @@
   </si>
   <si>
     <t>2016</t>
+  </si>
+  <si>
+    <t>Invalidemail</t>
+  </si>
+  <si>
+    <t>rafishaik.m@imimobile</t>
+  </si>
+  <si>
+    <t>Invalid Email</t>
+  </si>
+  <si>
+    <t>Invalid Email confirmation</t>
+  </si>
+  <si>
+    <t>Emptyemail_forgotpassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
   </si>
 </sst>
 </file>
@@ -448,7 +469,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy&quot; &quot;hh&quot;:&quot;mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,6 +525,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -526,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -599,6 +635,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1023,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1036,9 +1074,12 @@
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1095,20 @@
       <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -1070,15 +1123,28 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2" location="!/registration/login"/>
+    <hyperlink ref="F2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1330,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -1463,7 +1529,7 @@
       </c>
       <c r="M2" s="32">
         <f ca="1">NOW()+3</f>
-        <v>44112.386366782404</v>
+        <v>44113.529328124998</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>11</v>

</xml_diff>